<commit_message>
Author= Pushkar shukla comment= Updated Burnt hours in taskbreakdown excel sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
+++ b/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
@@ -351,24 +351,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,6 +367,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,7 +697,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,10 +734,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="39">
         <v>14</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -749,14 +749,17 @@
       <c r="E3" s="20">
         <v>2</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
       <c r="G3" s="20">
-        <v>2</v>
+        <f>(E3-F3)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -766,14 +769,17 @@
       <c r="E4" s="22">
         <v>1</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
       <c r="G4" s="22">
-        <v>1</v>
+        <f>(E4-F4)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
@@ -783,14 +789,17 @@
       <c r="E5" s="21">
         <v>4</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="16">
+        <v>3</v>
+      </c>
       <c r="G5" s="21">
-        <v>4</v>
+        <f>(E5-F5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
@@ -806,8 +815,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
@@ -823,8 +832,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
@@ -840,8 +849,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
@@ -857,25 +866,25 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="38" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="40">
-        <v>1</v>
-      </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41">
+      <c r="E10" s="34">
+        <v>1</v>
+      </c>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
@@ -891,19 +900,19 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="42" t="s">
+      <c r="A12" s="44"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="42">
-        <v>1</v>
-      </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="44">
+      <c r="E12" s="36">
+        <v>1</v>
+      </c>
+      <c r="F12" s="36"/>
+      <c r="G12" s="38">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author : Pushkar shukla comment : burnt hour updated in PushkarShukla.xlsx.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
+++ b/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
@@ -697,7 +697,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,11 +790,11 @@
         <v>4</v>
       </c>
       <c r="F5" s="16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5" s="21">
         <f>(E5-F5)</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -809,7 +809,9 @@
       <c r="E6" s="23">
         <v>1</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="23">
+        <v>1</v>
+      </c>
       <c r="G6" s="27">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Author : Pushkar shukla Comment: TasksBreakDown/PushkarShukla.xlsx,excel sheet updated.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
+++ b/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>test master sql or dummy schema</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>in Dev</t>
   </si>
 </sst>
 </file>
@@ -134,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +216,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -272,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,6 +400,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +759,7 @@
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -732,8 +781,11 @@
       <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
@@ -746,18 +798,21 @@
       <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="45">
         <v>2</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="20">
         <v>2</v>
       </c>
       <c r="G3" s="20">
         <f>(E3-F3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" s="40"/>
       <c r="C4" s="4" t="s">
@@ -766,18 +821,21 @@
       <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="22">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="46">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22">
         <v>1</v>
       </c>
       <c r="G4" s="22">
         <f>(E4-F4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" s="40"/>
       <c r="C5" s="16" t="s">
@@ -786,18 +844,21 @@
       <c r="D5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="47">
         <v>4</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="47">
         <v>6</v>
       </c>
       <c r="G5" s="21">
         <f>(E5-F5)</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" s="40"/>
       <c r="C6" s="18" t="s">
@@ -806,7 +867,7 @@
       <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="48">
         <v>1</v>
       </c>
       <c r="F6" s="23">
@@ -815,8 +876,9 @@
       <c r="G6" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="56"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="40"/>
       <c r="C7" s="5" t="s">
@@ -825,15 +887,16 @@
       <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="49">
         <v>1</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="40"/>
       <c r="C8" s="12" t="s">
@@ -842,15 +905,16 @@
       <c r="D8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="50">
         <v>1</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="29">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="43"/>
       <c r="B9" s="40"/>
       <c r="C9" s="6" t="s">
@@ -859,15 +923,16 @@
       <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="51">
         <v>1</v>
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="30">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="40"/>
       <c r="C10" s="32" t="s">
@@ -876,15 +941,16 @@
       <c r="D10" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="52">
         <v>1</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="40"/>
       <c r="C11" s="5" t="s">
@@ -893,15 +959,16 @@
       <c r="D11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="49">
         <v>1</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="41"/>
       <c r="C12" s="36" t="s">
@@ -910,26 +977,35 @@
       <c r="D12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="53">
         <v>1</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="38">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="31">
+        <f>SUM(E3:E12)</f>
+        <v>14</v>
+      </c>
+      <c r="F13" s="31">
+        <f>SUM(F3:F12)</f>
+        <v>10</v>
+      </c>
       <c r="G13" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(G2:G12)</f>
+        <v>5</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -939,8 +1015,9 @@
       <c r="G14" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -950,8 +1027,9 @@
       <c r="G15" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -961,8 +1039,9 @@
       <c r="G16" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -972,8 +1051,9 @@
       <c r="G17" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -984,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -995,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1006,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1017,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1028,7 +1108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1039,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1050,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1061,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1072,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1083,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1094,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1105,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1116,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1127,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1291,9 +1371,10 @@
       <c r="G46" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:B12"/>
     <mergeCell ref="A3:A12"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author: Pushkar Comment: TasksBreakDown excel sheet updated.
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
+++ b/TeamDetails/TasksBreakDown/PushkarShukla.xlsx
@@ -383,6 +383,37 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -401,37 +432,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,16 +781,17 @@
       <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="48" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39">
-        <v>14</v>
+      <c r="B3" s="50">
+        <f>SUM(E3:E12)</f>
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>8</v>
@@ -798,7 +799,7 @@
       <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="39">
         <v>2</v>
       </c>
       <c r="F3" s="20">
@@ -808,20 +809,20 @@
         <f>(E3-F3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="55" t="s">
+      <c r="H3" s="49" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="40">
         <v>1</v>
       </c>
       <c r="F4" s="22">
@@ -831,23 +832,23 @@
         <f>(E4-F4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="49" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="41">
         <v>4</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="41">
         <v>6</v>
       </c>
       <c r="G5" s="21">
@@ -859,19 +860,19 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="48">
-        <v>1</v>
+      <c r="E6" s="42">
+        <v>17</v>
       </c>
       <c r="F6" s="23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G6" s="27">
         <v>1</v>
@@ -879,15 +880,15 @@
       <c r="H6" s="56"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="43">
         <v>1</v>
       </c>
       <c r="F7" s="24"/>
@@ -897,15 +898,15 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="44">
         <v>1</v>
       </c>
       <c r="F8" s="25"/>
@@ -915,15 +916,15 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="45">
         <v>1</v>
       </c>
       <c r="F9" s="26"/>
@@ -933,15 +934,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="46">
         <v>1</v>
       </c>
       <c r="F10" s="34"/>
@@ -951,15 +952,15 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="40"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="43">
         <v>1</v>
       </c>
       <c r="F11" s="5"/>
@@ -969,15 +970,15 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="36" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="47">
         <v>1</v>
       </c>
       <c r="F12" s="36"/>
@@ -993,11 +994,11 @@
       <c r="D13" s="3"/>
       <c r="E13" s="31">
         <f>SUM(E3:E12)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F13" s="31">
         <f>SUM(F3:F12)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G13" s="31">
         <f>SUM(G2:G12)</f>

</xml_diff>